<commit_message>
implemented login and table to the app
</commit_message>
<xml_diff>
--- a/server/brokers_submissions/test.xlsx
+++ b/server/brokers_submissions/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BLASRS-External-App\BLASRS-External\server\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CB9D5A-D475-49A6-94E6-FF94CA376CE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34658F6-5863-455F-98BE-A9D5564F80DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5031,12 +5031,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5046,11 +5040,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5395,7 +5395,7 @@
   <dimension ref="A1:D917"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5408,30 +5408,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>1590</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>1593</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>1592</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="20" t="s">
         <v>1594</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="16" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>1591</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="23">
         <v>123456</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="22">
         <v>45016</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="21">
         <v>45031</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added guards and resolved pending issues
</commit_message>
<xml_diff>
--- a/server/brokers_submissions/test.xlsx
+++ b/server/brokers_submissions/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BLASRS-External-App\BLASRS-External\server\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammad.hassan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34658F6-5863-455F-98BE-A9D5564F80DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C70D65-C833-4F9A-92B5-663902F1E9CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5395,7 +5395,7 @@
   <dimension ref="A1:D917"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5429,7 +5429,7 @@
         <v>123456</v>
       </c>
       <c r="C2" s="22">
-        <v>45016</v>
+        <v>45046</v>
       </c>
       <c r="D2" s="21">
         <v>45031</v>

</xml_diff>